<commit_message>
Added photo and GLM 0.9.4.6 release
</commit_message>
<xml_diff>
--- a/doc/OpenGL matrix.xlsx
+++ b/doc/OpenGL matrix.xlsx
@@ -4463,6 +4463,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -9650,8 +9651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O251"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="Q143" sqref="Q143"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12056,10 +12057,10 @@
       <c r="D74" s="64" t="s">
         <v>163</v>
       </c>
-      <c r="E74" s="64" t="s">
-        <v>163</v>
-      </c>
-      <c r="F74" s="63" t="s">
+      <c r="E74" s="65" t="s">
+        <v>138</v>
+      </c>
+      <c r="F74" s="65" t="s">
         <v>138</v>
       </c>
       <c r="G74" s="64" t="s">
@@ -13377,7 +13378,7 @@
       </c>
       <c r="E102" s="6">
         <f t="shared" si="11"/>
-        <v>0.58695652173913049</v>
+        <v>0.60869565217391308</v>
       </c>
       <c r="F102" s="6">
         <f t="shared" si="11"/>
@@ -20431,7 +20432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O230"/>
   <sheetViews>
-    <sheetView topLeftCell="A109" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added photo 40 and 41
</commit_message>
<xml_diff>
--- a/doc/OpenGL matrix.xlsx
+++ b/doc/OpenGL matrix.xlsx
@@ -201,7 +201,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17005" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17005" uniqueCount="276">
   <si>
     <t>Fermi</t>
   </si>
@@ -1013,9 +1013,6 @@
     <t>OpenGL Matrix - November 2013</t>
   </si>
   <si>
-    <t>13.10 beta 1</t>
-  </si>
-  <si>
     <t>331.10 beta</t>
   </si>
   <si>
@@ -1023,6 +1020,15 @@
   </si>
   <si>
     <t>HSW</t>
+  </si>
+  <si>
+    <t>git-10.0</t>
+  </si>
+  <si>
+    <t>10.9</t>
+  </si>
+  <si>
+    <t>13.11 beta 8</t>
   </si>
 </sst>
 </file>
@@ -2742,7 +2748,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.2857142857142857</c:v>
+                  <c:v>0.38095238095238093</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.58333333333333337</c:v>
@@ -2757,7 +2763,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.88888888888888884</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1</c:v>
@@ -2890,11 +2896,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="559339520"/>
-        <c:axId val="130784576"/>
+        <c:axId val="103148544"/>
+        <c:axId val="56925504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="559339520"/>
+        <c:axId val="103148544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2903,7 +2909,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="130784576"/>
+        <c:crossAx val="56925504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2911,7 +2917,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="130784576"/>
+        <c:axId val="56925504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2923,7 +2929,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="559339520"/>
+        <c:crossAx val="103148544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4458,11 +4464,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="561544704"/>
-        <c:axId val="560095808"/>
+        <c:axId val="106549760"/>
+        <c:axId val="103031360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="561544704"/>
+        <c:axId val="106549760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4471,7 +4477,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="560095808"/>
+        <c:crossAx val="103031360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4479,7 +4485,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="560095808"/>
+        <c:axId val="103031360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4491,7 +4497,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="561544704"/>
+        <c:crossAx val="106549760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6025,11 +6031,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="561717760"/>
-        <c:axId val="560101568"/>
+        <c:axId val="107353600"/>
+        <c:axId val="103037120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="561717760"/>
+        <c:axId val="107353600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6038,7 +6044,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="560101568"/>
+        <c:crossAx val="103037120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6046,7 +6052,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="560101568"/>
+        <c:axId val="103037120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -6058,7 +6064,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="561717760"/>
+        <c:crossAx val="107353600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7592,11 +7598,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="562869760"/>
-        <c:axId val="560102720"/>
+        <c:axId val="107207680"/>
+        <c:axId val="103038272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="562869760"/>
+        <c:axId val="107207680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7605,7 +7611,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="560102720"/>
+        <c:crossAx val="103038272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7613,7 +7619,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="560102720"/>
+        <c:axId val="103038272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -7625,7 +7631,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="562869760"/>
+        <c:crossAx val="107207680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9159,11 +9165,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="563421696"/>
-        <c:axId val="562811968"/>
+        <c:axId val="108758528"/>
+        <c:axId val="107123776"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="563421696"/>
+        <c:axId val="108758528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9172,7 +9178,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="562811968"/>
+        <c:crossAx val="107123776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9180,7 +9186,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="562811968"/>
+        <c:axId val="107123776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -9192,7 +9198,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="563421696"/>
+        <c:crossAx val="108758528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10726,11 +10732,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="564172288"/>
-        <c:axId val="562813120"/>
+        <c:axId val="108514304"/>
+        <c:axId val="107124928"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="564172288"/>
+        <c:axId val="108514304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10739,7 +10745,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="562813120"/>
+        <c:crossAx val="107124928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10747,7 +10753,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="562813120"/>
+        <c:axId val="107124928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -10759,7 +10765,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="564172288"/>
+        <c:crossAx val="108514304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11289,8 +11295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P251"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A226" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M241" sqref="M241:N241"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11473,14 +11479,14 @@
         <v>176</v>
       </c>
       <c r="B9" s="75" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C9" s="75"/>
       <c r="D9" s="75"/>
       <c r="E9" s="75"/>
       <c r="F9" s="75"/>
       <c r="G9" s="75" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="H9" s="75"/>
       <c r="I9" s="75"/>
@@ -11494,10 +11500,10 @@
         <v>3277</v>
       </c>
       <c r="O9" s="69" t="s">
-        <v>241</v>
+        <v>273</v>
       </c>
       <c r="P9" s="69" t="s">
-        <v>266</v>
+        <v>274</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11512,7 +11518,7 @@
       <c r="E10" s="71"/>
       <c r="F10" s="71"/>
       <c r="G10" s="70">
-        <v>41553</v>
+        <v>41577</v>
       </c>
       <c r="H10" s="71"/>
       <c r="I10" s="71"/>
@@ -11526,10 +11532,10 @@
         <v>41516</v>
       </c>
       <c r="O10" s="66">
-        <v>41363</v>
+        <v>41584</v>
       </c>
       <c r="P10" s="51">
-        <v>41347</v>
+        <v>41569</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -11570,10 +11576,10 @@
         <v>165</v>
       </c>
       <c r="M11" s="38" t="s">
+        <v>271</v>
+      </c>
+      <c r="N11" s="38" t="s">
         <v>272</v>
-      </c>
-      <c r="N11" s="38" t="s">
-        <v>273</v>
       </c>
       <c r="O11" s="38" t="s">
         <v>218</v>
@@ -11705,7 +11711,7 @@
       </c>
       <c r="O13" s="40">
         <f t="shared" si="1"/>
-        <v>0.2857142857142857</v>
+        <v>0.38095238095238093</v>
       </c>
       <c r="P13" s="40">
         <f t="shared" si="1"/>
@@ -12030,7 +12036,7 @@
       </c>
       <c r="O18" s="40">
         <f t="shared" si="6"/>
-        <v>0.88888888888888884</v>
+        <v>1</v>
       </c>
       <c r="P18" s="40">
         <f t="shared" si="6"/>
@@ -12919,10 +12925,10 @@
         <v>165</v>
       </c>
       <c r="M55" s="33" t="s">
+        <v>271</v>
+      </c>
+      <c r="N55" s="33" t="s">
         <v>272</v>
-      </c>
-      <c r="N55" s="33" t="s">
-        <v>273</v>
       </c>
       <c r="O55" s="33" t="s">
         <v>218</v>
@@ -15352,10 +15358,10 @@
         <v>165</v>
       </c>
       <c r="M104" s="33" t="s">
+        <v>271</v>
+      </c>
+      <c r="N104" s="33" t="s">
         <v>272</v>
-      </c>
-      <c r="N104" s="33" t="s">
-        <v>273</v>
       </c>
       <c r="O104" s="33" t="s">
         <v>218</v>
@@ -15885,10 +15891,10 @@
         <v>165</v>
       </c>
       <c r="M115" s="33" t="s">
+        <v>271</v>
+      </c>
+      <c r="N115" s="33" t="s">
         <v>272</v>
-      </c>
-      <c r="N115" s="33" t="s">
-        <v>273</v>
       </c>
       <c r="O115" s="33" t="s">
         <v>218</v>
@@ -15940,8 +15946,8 @@
       <c r="N116" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="O116" s="4" t="s">
-        <v>163</v>
+      <c r="O116" s="56" t="s">
+        <v>138</v>
       </c>
       <c r="P116" s="4" t="s">
         <v>163</v>
@@ -15990,8 +15996,8 @@
       <c r="N117" s="64" t="s">
         <v>163</v>
       </c>
-      <c r="O117" s="64" t="s">
-        <v>163</v>
+      <c r="O117" s="65" t="s">
+        <v>138</v>
       </c>
       <c r="P117" s="64" t="s">
         <v>163</v>
@@ -17005,7 +17011,7 @@
       </c>
       <c r="O137" s="6">
         <f t="shared" si="13"/>
-        <v>0.2857142857142857</v>
+        <v>0.38095238095238093</v>
       </c>
       <c r="P137" s="6">
         <f t="shared" si="13"/>
@@ -17068,10 +17074,10 @@
         <v>165</v>
       </c>
       <c r="M139" s="33" t="s">
+        <v>271</v>
+      </c>
+      <c r="N139" s="33" t="s">
         <v>272</v>
-      </c>
-      <c r="N139" s="33" t="s">
-        <v>273</v>
       </c>
       <c r="O139" s="33" t="s">
         <v>218</v>
@@ -17801,10 +17807,10 @@
         <v>165</v>
       </c>
       <c r="M154" s="33" t="s">
+        <v>271</v>
+      </c>
+      <c r="N154" s="33" t="s">
         <v>272</v>
-      </c>
-      <c r="N154" s="33" t="s">
-        <v>273</v>
       </c>
       <c r="O154" s="33" t="s">
         <v>218</v>
@@ -18234,10 +18240,10 @@
         <v>165</v>
       </c>
       <c r="M163" s="33" t="s">
+        <v>271</v>
+      </c>
+      <c r="N163" s="33" t="s">
         <v>272</v>
-      </c>
-      <c r="N163" s="33" t="s">
-        <v>273</v>
       </c>
       <c r="O163" s="33" t="s">
         <v>218</v>
@@ -19017,10 +19023,10 @@
         <v>165</v>
       </c>
       <c r="M179" s="33" t="s">
+        <v>271</v>
+      </c>
+      <c r="N179" s="33" t="s">
         <v>272</v>
-      </c>
-      <c r="N179" s="33" t="s">
-        <v>273</v>
       </c>
       <c r="O179" s="33" t="s">
         <v>218</v>
@@ -19650,10 +19656,10 @@
         <v>165</v>
       </c>
       <c r="M192" s="33" t="s">
+        <v>271</v>
+      </c>
+      <c r="N192" s="33" t="s">
         <v>272</v>
-      </c>
-      <c r="N192" s="33" t="s">
-        <v>273</v>
       </c>
       <c r="O192" s="33" t="s">
         <v>218</v>
@@ -19955,8 +19961,8 @@
       <c r="N198" s="63" t="s">
         <v>138</v>
       </c>
-      <c r="O198" s="64" t="s">
-        <v>163</v>
+      <c r="O198" s="65" t="s">
+        <v>138</v>
       </c>
       <c r="P198" s="63" t="s">
         <v>138</v>
@@ -20170,7 +20176,7 @@
       </c>
       <c r="O202" s="21">
         <f t="shared" si="18"/>
-        <v>0.88888888888888884</v>
+        <v>1</v>
       </c>
       <c r="P202" s="21">
         <f t="shared" si="18"/>
@@ -20233,10 +20239,10 @@
         <v>165</v>
       </c>
       <c r="M204" s="33" t="s">
+        <v>271</v>
+      </c>
+      <c r="N204" s="33" t="s">
         <v>272</v>
-      </c>
-      <c r="N204" s="33" t="s">
-        <v>273</v>
       </c>
       <c r="O204" s="33" t="s">
         <v>218</v>
@@ -20716,10 +20722,10 @@
         <v>165</v>
       </c>
       <c r="M214" s="33" t="s">
+        <v>271</v>
+      </c>
+      <c r="N214" s="33" t="s">
         <v>272</v>
-      </c>
-      <c r="N214" s="33" t="s">
-        <v>273</v>
       </c>
       <c r="O214" s="33" t="s">
         <v>218</v>
@@ -21799,10 +21805,10 @@
         <v>165</v>
       </c>
       <c r="M236" s="33" t="s">
+        <v>271</v>
+      </c>
+      <c r="N236" s="33" t="s">
         <v>272</v>
-      </c>
-      <c r="N236" s="33" t="s">
-        <v>273</v>
       </c>
       <c r="O236" s="33" t="s">
         <v>218</v>
@@ -22032,10 +22038,10 @@
         <v>165</v>
       </c>
       <c r="M241" s="33" t="s">
+        <v>271</v>
+      </c>
+      <c r="N241" s="33" t="s">
         <v>272</v>
-      </c>
-      <c r="N241" s="33" t="s">
-        <v>273</v>
       </c>
       <c r="O241" s="33" t="s">
         <v>218</v>
@@ -22744,7 +22750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O251"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
+    <sheetView topLeftCell="A58" workbookViewId="0">
       <selection activeCell="R129" sqref="R129"/>
     </sheetView>
   </sheetViews>

</xml_diff>